<commit_message>
added functional tests, .gitignores, cleanup
</commit_message>
<xml_diff>
--- a/test/Test1.xlsx
+++ b/test/Test1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhushon/go/src/decxls/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71D30CAF-5AD8-2E40-A812-08903C921A76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E477D91B-9B2D-DC42-8ED1-503D21667320}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{9CC7F51F-F904-464C-AD39-B1BBC74373DC}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -431,7 +431,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="1">
-        <v>13</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -442,7 +442,7 @@
         <v>22</v>
       </c>
       <c r="C3" s="1">
-        <v>23</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -453,7 +453,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="1">
-        <v>33</v>
+        <v>3.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated tests, readme and eliminated dead code
</commit_message>
<xml_diff>
--- a/test/Test1.xlsx
+++ b/test/Test1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhushon/go/src/decxls/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E477D91B-9B2D-DC42-8ED1-503D21667320}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A874A8F8-C590-F444-BCBE-69EE068DBFD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{9CC7F51F-F904-464C-AD39-B1BBC74373DC}"/>
+    <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{9CC7F51F-F904-464C-AD39-B1BBC74373DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>Header 1</t>
   </si>
@@ -406,8 +407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16A71FDB-6D87-B442-9F19-0A30C0511232}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -459,4 +460,63 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9017FAFA-1959-014F-9A66-F7EEE5B89F09}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="C4">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>